<commit_message>
Created a loop for excess returns for the indices
</commit_message>
<xml_diff>
--- a/Thesis/Literature.Review/data/Literature Summary Table.xlsx
+++ b/Thesis/Literature.Review/data/Literature Summary Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielrambanapasi/Desktop/Much Ado Dividends/Much-Ado-Dividends/Literature.Review/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielrambanapasi/Desktop/Much Ado Dividends/Much-Ado-Dividends/Thesis/Literature.Review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A04261C-1E8B-EF40-9EFD-D7EE0CBB5817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F164571-A67B-3C4E-98DF-60B245522556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{F79D501E-F1A1-9443-9865-2BE103D0438B}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>Signal</t>
   </si>
   <si>
-    <t xml:space="preserve">Dividend portfolio outperformed market index. </t>
-  </si>
-  <si>
     <t>High Dividend Yield</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">Result </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outperformed market index </t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +476,7 @@
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="143.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -493,7 +493,7 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -507,10 +507,10 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -524,10 +524,10 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -541,10 +541,10 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -558,10 +558,10 @@
         <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -575,10 +575,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -592,10 +592,10 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -609,10 +609,10 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -626,10 +626,10 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -643,10 +643,10 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -660,10 +660,10 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strat done now rolling standard dev
</commit_message>
<xml_diff>
--- a/Thesis/Literature.Review/data/Literature Summary Table.xlsx
+++ b/Thesis/Literature.Review/data/Literature Summary Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielrambanapasi/Desktop/Much Ado Dividends/Much-Ado-Dividends/Thesis/Literature.Review/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F164571-A67B-3C4E-98DF-60B245522556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BF9866-7D79-634F-85E2-B1C4D6A1B393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" xr2:uid="{F79D501E-F1A1-9443-9865-2BE103D0438B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t xml:space="preserve">Year </t>
   </si>
@@ -56,9 +56,6 @@
     <t>Filbeck</t>
   </si>
   <si>
-    <t xml:space="preserve">Optimiization </t>
-  </si>
-  <si>
     <t xml:space="preserve">Lemmon </t>
   </si>
   <si>
@@ -74,33 +71,6 @@
     <t>Brzeszczyński</t>
   </si>
   <si>
-    <t>Geography</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brazil </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poland </t>
-  </si>
-  <si>
-    <t xml:space="preserve">US </t>
-  </si>
-  <si>
-    <t xml:space="preserve">China </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hong Kong </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taiwan </t>
-  </si>
-  <si>
     <t>Signal</t>
   </si>
   <si>
@@ -110,10 +80,10 @@
     <t xml:space="preserve">Dividend Growth </t>
   </si>
   <si>
-    <t xml:space="preserve">Result </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outperformed market index </t>
+    <t>Methodology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grouped high yield stock and tests for yield effect at portfolio level.  Fama-MacBeth methodology and tests for yield effect after controlling for known factors. </t>
   </si>
 </sst>
 </file>
@@ -465,21 +435,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8E8D45-18D3-0349-88EF-B40FE2BEE037}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,16 +456,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1997</v>
       </c>
@@ -504,16 +470,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2001</v>
       </c>
@@ -521,16 +481,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2003</v>
       </c>
@@ -538,50 +492,32 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2007</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2007</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2011</v>
       </c>
@@ -589,50 +525,35 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2011</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2015</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2017</v>
       </c>
@@ -640,34 +561,22 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D11">
     <sortCondition ref="A2:A11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>